<commit_message>
Update summary data file with corrected column name
</commit_message>
<xml_diff>
--- a/public/Summary RMT Rev & Expense Data for Dashboard.xlsx
+++ b/public/Summary RMT Rev & Expense Data for Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9705D4F-6AC9-4A4A-B11D-935E449DF6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38E366C-075D-A641-963C-A3E6C9429545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="2460" windowWidth="25800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="440" yWindow="760" windowWidth="28280" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YOY Rev &amp; Visits" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>Expenses 2024</t>
   </si>
   <si>
-    <t>Expensese 2025</t>
-  </si>
-  <si>
     <t>2024 Profit</t>
   </si>
   <si>
@@ -83,6 +80,9 @@
   </si>
   <si>
     <t>% YOY Change</t>
+  </si>
+  <si>
+    <t>Expenses 2025</t>
   </si>
 </sst>
 </file>
@@ -92,7 +92,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -125,6 +125,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -143,10 +150,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -162,9 +170,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -383,7 +395,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -408,45 +420,45 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3">
         <v>146886.78</v>
@@ -457,7 +469,7 @@
       <c r="D2" s="3">
         <v>-5392.7300000000105</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="7">
         <v>-3.6713514994337886E-2</v>
       </c>
       <c r="F2" s="3">
@@ -496,7 +508,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3">
         <v>106956.59</v>
@@ -507,7 +519,7 @@
       <c r="D3" s="3">
         <v>7728.4100000000035</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="7">
         <v>7.2257445754394412E-2</v>
       </c>
       <c r="F3" s="3">
@@ -546,7 +558,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3">
         <v>78767.17</v>
@@ -557,7 +569,7 @@
       <c r="D4" s="3">
         <v>65323.009999999995</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="7">
         <v>0.82931772209157695</v>
       </c>
       <c r="F4" s="3">
@@ -596,7 +608,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3">
         <v>89056.75</v>
@@ -607,7 +619,7 @@
       <c r="D5" s="3">
         <v>58024.290000000008</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="7">
         <v>0.65154286452177979</v>
       </c>
       <c r="F5" s="3">
@@ -646,7 +658,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3">
         <v>106934.98</v>
@@ -657,7 +669,7 @@
       <c r="D6" s="3">
         <v>-25540.92</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="7">
         <v>-0.23884532451401777</v>
       </c>
       <c r="F6" s="3">
@@ -696,7 +708,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3">
         <v>88672.17</v>
@@ -707,7 +719,7 @@
       <c r="D7" s="3">
         <v>49456.83</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="7">
         <v>0.55774917880096997</v>
       </c>
       <c r="F7" s="3">
@@ -746,7 +758,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3">
         <v>617274.44000000006</v>
@@ -757,7 +769,7 @@
       <c r="D8" s="3">
         <v>149598.89000000001</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="7">
         <v>0.24235393579555958</v>
       </c>
       <c r="F8" s="3">

</xml_diff>

<commit_message>
Update summary data file with latest local changes
</commit_message>
<xml_diff>
--- a/public/Summary RMT Rev & Expense Data for Dashboard.xlsx
+++ b/public/Summary RMT Rev & Expense Data for Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38E366C-075D-A641-963C-A3E6C9429545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9932B27-0360-CF42-8F14-99C5AFA21B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="28280" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Month</t>
   </si>
@@ -79,10 +79,13 @@
     <t>2024 Total Vists</t>
   </si>
   <si>
-    <t>% YOY Change</t>
-  </si>
-  <si>
     <t>Expenses 2025</t>
+  </si>
+  <si>
+    <t>% YOY Expenses Change</t>
+  </si>
+  <si>
+    <t>% YOY Revenue Change</t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -420,19 +423,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update section and column titles for Expense Trends Over Entire Dataset and new column names
</commit_message>
<xml_diff>
--- a/public/Summary RMT Rev & Expense Data for Dashboard.xlsx
+++ b/public/Summary RMT Rev & Expense Data for Dashboard.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9932B27-0360-CF42-8F14-99C5AFA21B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02C864C-085C-804D-B87E-99BEAFFA9F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="28280" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YOY Rev &amp; Visits" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -398,13 +411,14 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="3" width="11.6640625" customWidth="1"/>
     <col min="6" max="7" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.5" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="18.6640625" customWidth="1"/>
     <col min="16" max="16" width="14.5" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>